<commit_message>
Updated with all figure data from Broggini, Duckworth, et al. 2024. NWB creation script is operational.
</commit_message>
<xml_diff>
--- a/Matlab/input_widefield_2P.xlsx
+++ b/Matlab/input_widefield_2P.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Jacob\nwb_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1981C5F-DF16-4FBF-A7CC-9E8A09831CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10657F8B-3A72-44A9-BFE7-F9B884CB6A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="114">
   <si>
     <t>session_id</t>
   </si>
@@ -110,9 +110,6 @@
     <t>B6.Cg-Gt(ROSA)26Sortm2.2Ksvo/J x Tg(PDGFRβ-cre)35Vli</t>
   </si>
   <si>
-    <t>Fig S4</t>
-  </si>
-  <si>
     <t>Duckworth, Jacob</t>
   </si>
   <si>
@@ -140,18 +137,9 @@
     <t>WT11</t>
   </si>
   <si>
-    <t>Pericyte - ReaChR</t>
-  </si>
-  <si>
     <t>WT</t>
   </si>
   <si>
-    <t>Fig 2e, 2f, 2h</t>
-  </si>
-  <si>
-    <t>Fig 2e, 2f, 2h, 2c, 2d, 2a, 2b</t>
-  </si>
-  <si>
     <t>WT997</t>
   </si>
   <si>
@@ -173,12 +161,6 @@
     <t>IS264</t>
   </si>
   <si>
-    <t>Fig 1h, 1i, 1j</t>
-  </si>
-  <si>
-    <t>Fig 1c, 1d, 1e, 1f, 1g, 1h, 1i, 1j</t>
-  </si>
-  <si>
     <t>WT PA</t>
   </si>
   <si>
@@ -317,24 +299,6 @@
     <t>Wide-field fluorescent microscope</t>
   </si>
   <si>
-    <t>Fig 3d</t>
-  </si>
-  <si>
-    <t>Fig 4b, 4c, 4d, 4f</t>
-  </si>
-  <si>
-    <t>Fig 3c, 3d</t>
-  </si>
-  <si>
-    <t>Fig 2e, 2f, 2h, 5a, 5b</t>
-  </si>
-  <si>
-    <t>Fig 2e, 2f, 2h, 5b</t>
-  </si>
-  <si>
-    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c</t>
-  </si>
-  <si>
     <t>Fig S3d, S3e, S3f</t>
   </si>
   <si>
@@ -366,6 +330,57 @@
   </si>
   <si>
     <t>Optogenetic Stim Constant; Imaging Light</t>
+  </si>
+  <si>
+    <t>Fig 2e, 2f, 2h, 5b, S5</t>
+  </si>
+  <si>
+    <t>Fig 2e, 2f, 2h, S5</t>
+  </si>
+  <si>
+    <t>Fig 2e, 2f, 2h, 5a, 5b, S5</t>
+  </si>
+  <si>
+    <t>Fig 2e, 2f, 2h, 2c, 2d, 2a, 2b, S5</t>
+  </si>
+  <si>
+    <t>Fig S4c, S4d</t>
+  </si>
+  <si>
+    <t>Fig S4b, S4c, S4d</t>
+  </si>
+  <si>
+    <t>Fig 3c, 3d, S6a, S6b</t>
+  </si>
+  <si>
+    <t>Fig 3d, S6a, S6b</t>
+  </si>
+  <si>
+    <t>Fig 4b, 4c, 4d, 4f, S8b</t>
+  </si>
+  <si>
+    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c, S8b</t>
+  </si>
+  <si>
+    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c, 6f, S7a, S7b, S7c, S8b</t>
+  </si>
+  <si>
+    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c 6f, S7a, S7b, S7c, S8b</t>
+  </si>
+  <si>
+    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c,  6f, S7a, S7b, S7c, S8b</t>
+  </si>
+  <si>
+    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c, 6b, 6c, 6d, 6e, 6f, S7a, S7b, S7c, S6c, S8b, S8c</t>
+  </si>
+  <si>
+    <t>Fig 1h, 1i, 1j, S2a, S2b, S2c, S2d, S2e, S2f, S2g, S2h</t>
+  </si>
+  <si>
+    <t>Fig 1c, 1d, 1e, 1f, 1g, 1h, 1i, 1j, S2a, S2b, S2c, S2d, S2e, S2f, S2g, S2h</t>
+  </si>
+  <si>
+    <t>Pericyte ReaChR</t>
   </si>
 </sst>
 </file>
@@ -885,9 +900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L6" sqref="L6"/>
+      <selection pane="topRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +917,9 @@
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="13" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33.5703125" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -963,16 +980,16 @@
         <v>18</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="W1" s="2"/>
       <c r="Z1" s="3" t="s">
@@ -984,22 +1001,22 @@
     </row>
     <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="9">
         <v>76</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>14</v>
@@ -1011,48 +1028,48 @@
         <v>16</v>
       </c>
       <c r="J2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="11">
         <v>77</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>14</v>
@@ -1064,48 +1081,48 @@
         <v>16</v>
       </c>
       <c r="J3" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="11">
         <v>90</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>14</v>
@@ -1117,48 +1134,48 @@
         <v>16</v>
       </c>
       <c r="J4" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="R4" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="11">
         <v>73</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>14</v>
@@ -1173,45 +1190,45 @@
         <v>44894</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R5" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="11">
         <v>77</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>14</v>
@@ -1226,45 +1243,45 @@
         <v>44894</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="11">
         <v>85</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>14</v>
@@ -1279,45 +1296,45 @@
         <v>44894</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="11">
         <v>92</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>14</v>
@@ -1332,45 +1349,45 @@
         <v>44894</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Q8" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R8" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C9" s="11">
         <v>191</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>14</v>
@@ -1385,45 +1402,45 @@
         <v>45139</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" s="7">
         <v>192</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>14</v>
@@ -1438,45 +1455,45 @@
         <v>45139</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" s="9">
         <v>96</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>14</v>
@@ -1491,45 +1508,45 @@
         <v>45104</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="11">
         <v>92</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>14</v>
@@ -1544,45 +1561,45 @@
         <v>45104</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q12" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <v>106</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>14</v>
@@ -1597,45 +1614,45 @@
         <v>45104</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C14" s="9">
         <v>123</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>14</v>
@@ -1650,45 +1667,45 @@
         <v>44400</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15" s="11">
         <v>138</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>14</v>
@@ -1703,45 +1720,45 @@
         <v>44400</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R15" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="11">
         <v>139</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>14</v>
@@ -1756,45 +1773,45 @@
         <v>44400</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7">
         <v>91</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>14</v>
@@ -1809,25 +1826,25 @@
         <v>44438</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1841,13 +1858,13 @@
         <v>237</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
@@ -1862,25 +1879,25 @@
         <v>45069</v>
       </c>
       <c r="K18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="N18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1894,13 +1911,13 @@
         <v>246</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
@@ -1915,25 +1932,25 @@
         <v>45069</v>
       </c>
       <c r="K19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="N19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1947,13 +1964,13 @@
         <v>180</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>14</v>
@@ -1967,46 +1984,46 @@
       <c r="J20" s="16">
         <v>45099</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="N20" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C21" s="9">
         <v>184</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>14</v>
@@ -2021,45 +2038,45 @@
         <v>44906</v>
       </c>
       <c r="K21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="M21" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="P21" s="6" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C22" s="11">
         <v>231</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>14</v>
@@ -2074,45 +2091,45 @@
         <v>44918</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>85</v>
+        <v>104</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C23" s="7">
         <v>157</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>14</v>
@@ -2127,45 +2144,45 @@
         <v>44991</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>85</v>
+        <v>104</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P23" s="8" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q23" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R23" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C24" s="19">
         <v>121</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G24" s="19" t="s">
         <v>14</v>
@@ -2180,45 +2197,45 @@
         <v>43718</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="M24" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="N24" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q24" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R24" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="N24" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="O24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P24" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q24" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R24" s="19" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C25" s="22">
         <v>130</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>14</v>
@@ -2233,45 +2250,45 @@
         <v>44227</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="M25" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P25" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R25" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N25" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P25" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q25" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R25" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C26" s="22">
         <v>172</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G26" s="22" t="s">
         <v>14</v>
@@ -2286,45 +2303,45 @@
         <v>44184</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="M26" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N26" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q26" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R26" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N26" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O26" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P26" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q26" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R26" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C27" s="22">
         <v>49</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>14</v>
@@ -2339,45 +2356,45 @@
         <v>43861</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="M27" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P27" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q27" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R27" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N27" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O27" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P27" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q27" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R27" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C28" s="22">
         <v>158</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>14</v>
@@ -2392,45 +2409,45 @@
         <v>44081</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="M28" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P28" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q28" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R28" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N28" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P28" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q28" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R28" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C29" s="22">
         <v>48</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G29" s="22" t="s">
         <v>14</v>
@@ -2445,45 +2462,45 @@
         <v>43861</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="M29" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N29" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P29" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q29" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R29" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N29" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P29" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q29" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R29" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C30" s="22">
         <v>59</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G30" s="22" t="s">
         <v>14</v>
@@ -2498,45 +2515,45 @@
         <v>43718</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="M30" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N30" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P30" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q30" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R30" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N30" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P30" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q30" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R30" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C31" s="22">
         <v>62</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G31" s="22" t="s">
         <v>14</v>
@@ -2551,45 +2568,45 @@
         <v>43718</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="M31" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N31" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P31" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q31" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R31" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N31" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P31" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q31" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R31" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C32" s="10">
         <v>153</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>14</v>
@@ -2604,45 +2621,45 @@
         <v>44125</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="M32" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P32" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R32" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N32" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P32" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R32" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C33" s="10">
         <v>103</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>14</v>
@@ -2657,45 +2674,45 @@
         <v>43987</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M33" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N33" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R33" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N33" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P33" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R33" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C34" s="22">
         <v>92</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G34" s="22" t="s">
         <v>14</v>
@@ -2710,45 +2727,45 @@
         <v>43878</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="M34" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N34" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P34" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q34" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R34" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N34" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O34" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P34" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q34" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R34" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C35" s="10">
         <v>73</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>14</v>
@@ -2763,45 +2780,45 @@
         <v>43878</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M35" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R35" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N35" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P35" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R35" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C36" s="10">
         <v>366</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>14</v>
@@ -2816,45 +2833,45 @@
         <v>43920</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M36" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P36" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R36" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N36" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q36" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R36" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C37" s="10">
         <v>364</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>14</v>
@@ -2869,45 +2886,45 @@
         <v>43920</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M37" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P37" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R37" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N37" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O37" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P37" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q37" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R37" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C38" s="10">
         <v>192</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G38" s="10" t="s">
         <v>14</v>
@@ -2922,45 +2939,45 @@
         <v>44166</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M38" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P38" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R38" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N38" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O38" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q38" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R38" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C39" s="22">
         <v>177</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G39" s="22" t="s">
         <v>14</v>
@@ -2975,45 +2992,45 @@
         <v>44184</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="M39" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N39" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P39" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q39" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R39" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="N39" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="O39" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P39" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q39" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="R39" s="22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C40" s="10">
         <v>177</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G40" s="10" t="s">
         <v>14</v>
@@ -3028,45 +3045,45 @@
         <v>44185</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M40" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q40" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R40" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N40" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O40" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R40" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C41" s="10">
         <v>134</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>14</v>
@@ -3081,45 +3098,45 @@
         <v>44227</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M41" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N41" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O41" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P41" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q41" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R41" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N41" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O41" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q41" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R41" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C42" s="10">
         <v>116</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>14</v>
@@ -3134,45 +3151,45 @@
         <v>43974</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M42" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N42" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R42" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N42" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O42" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P42" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q42" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R42" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C43" s="10">
         <v>227</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>14</v>
@@ -3187,45 +3204,45 @@
         <v>43920</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M43" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N43" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P43" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R43" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N43" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O43" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q43" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R43" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C44" s="10">
         <v>227</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>14</v>
@@ -3240,45 +3257,45 @@
         <v>43920</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M44" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N44" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P44" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R44" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="N44" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O44" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="P44" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q44" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R44" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C45" s="10">
         <v>217</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>14</v>
@@ -3293,45 +3310,45 @@
         <v>44466</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M45" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N45" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P45" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q45" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="R45" s="10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C46" s="10">
         <v>223</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>14</v>
@@ -3346,45 +3363,45 @@
         <v>44485</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N46" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q46" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="R46" s="10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C47" s="8">
         <v>92</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>14</v>
@@ -3399,25 +3416,25 @@
         <v>44627</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="P47" s="8" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="Q47" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="R47" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Widefield_2P Excel file and MATLAB file to create nwb files to the versions used for 5/22/24 upload to DANDI Broggini, Duckworth et al.
</commit_message>
<xml_diff>
--- a/Matlab/input_widefield_2P.xlsx
+++ b/Matlab/input_widefield_2P.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Jacob\nwb_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10657F8B-3A72-44A9-BFE7-F9B884CB6A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2CCCE5-D6EF-40C4-A6C3-6484507EAFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="38640" windowHeight="23640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="auto" sheetId="1" r:id="rId1"/>
@@ -371,9 +371,6 @@
     <t>Fig 4b, 4c, 4d, 4e, 4f, 5c,  6f, S7a, S7b, S7c, S8b</t>
   </si>
   <si>
-    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c, 6b, 6c, 6d, 6e, 6f, S7a, S7b, S7c, S6c, S8b, S8c</t>
-  </si>
-  <si>
     <t>Fig 1h, 1i, 1j, S2a, S2b, S2c, S2d, S2e, S2f, S2g, S2h</t>
   </si>
   <si>
@@ -381,6 +378,9 @@
   </si>
   <si>
     <t>Pericyte ReaChR</t>
+  </si>
+  <si>
+    <t>Fig 4b, 4c, 4d, 4e, 4f, 5c, 6b, 6c, 6d, 6e, 6f, S7a, S7b, S7c, S6c, S8a, S8b, S8c</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G31" sqref="G31"/>
+      <selection pane="topRight" activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1667,7 @@
         <v>44400</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>87</v>
@@ -1720,7 +1720,7 @@
         <v>44400</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>87</v>
@@ -1773,7 +1773,7 @@
         <v>44400</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>87</v>
@@ -1826,7 +1826,7 @@
         <v>44438</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>87</v>
@@ -1858,7 +1858,7 @@
         <v>237</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>22</v>
@@ -1911,7 +1911,7 @@
         <v>246</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>22</v>
@@ -1964,7 +1964,7 @@
         <v>180</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>22</v>
@@ -2356,7 +2356,7 @@
         <v>43861</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="M27" s="22" t="s">
         <v>79</v>

</xml_diff>